<commit_message>
First pass of implementing rigid body physics
</commit_message>
<xml_diff>
--- a/doc/Research/BSP Layout.xlsx
+++ b/doc/Research/BSP Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\source\openh2\doc\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209C5A8-76DA-478E-A77C-2F6FFC69BBE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CA78EC-F324-4088-95AF-3ABCD37AB0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30375" yWindow="345" windowWidth="26160" windowHeight="13995" firstSheet="2" activeTab="2" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="116">
   <si>
     <t>File size</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>Sec magic</t>
+  </si>
+  <si>
+    <t>node, left, right</t>
   </si>
 </sst>
 </file>
@@ -2033,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5402844C-0554-4902-B07C-5C11243F8396}">
-  <dimension ref="A1:K116"/>
+  <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2055,7 @@
     <col min="10" max="10" width="72.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>0.99945142230196915</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>37</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>3</v>
@@ -2110,7 +2113,7 @@
       <c r="I4" s="17"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -2136,7 +2139,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>38</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>3</v>
@@ -2172,7 +2175,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -2198,7 +2201,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>1</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>3</v>
@@ -2243,8 +2246,11 @@
       <c r="J15" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>4</v>
@@ -4138,11 +4144,11 @@
         <v>912</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E30" si="2">D3 +42332576</f>
+        <f t="shared" ref="E3:E27" si="2">D3 +42332576</f>
         <v>42333488</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F30" si="3">(D4-D3)/C3</f>
+        <f t="shared" ref="F3:F27" si="3">(D4-D3)/C3</f>
         <v>515540</v>
       </c>
       <c r="G3" s="25" t="s">
@@ -4868,7 +4874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AD3F75-2402-4656-A232-23962ACADB26}">
   <dimension ref="B1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>

</xml_diff>